<commit_message>
Corrected web scraping bugs
</commit_message>
<xml_diff>
--- a/financial_files/excel/AMZN.xlsx
+++ b/financial_files/excel/AMZN.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="financial_data_scraped" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="financial_statement_api" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="rule1_results" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -156,6 +158,47 @@
     <tableColumn id="13" name="2018"/>
     <tableColumn id="14" name="2019"/>
     <tableColumn id="15" name="TTM"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="financial_statement_api" displayName="financial_statement_api" ref="A1:U23" headerRowCount="1">
+  <autoFilter ref="A1:U23"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="API Parameter"/>
+    <tableColumn id="2" name="2000"/>
+    <tableColumn id="3" name="2001"/>
+    <tableColumn id="4" name="2002"/>
+    <tableColumn id="5" name="2003"/>
+    <tableColumn id="6" name="2004"/>
+    <tableColumn id="7" name="2005"/>
+    <tableColumn id="8" name="2006"/>
+    <tableColumn id="9" name="2007"/>
+    <tableColumn id="10" name="2008"/>
+    <tableColumn id="11" name="2009"/>
+    <tableColumn id="12" name="2010"/>
+    <tableColumn id="13" name="2011"/>
+    <tableColumn id="14" name="2012"/>
+    <tableColumn id="15" name="2013"/>
+    <tableColumn id="16" name="2014"/>
+    <tableColumn id="17" name="2015"/>
+    <tableColumn id="18" name="2016"/>
+    <tableColumn id="19" name="2017"/>
+    <tableColumn id="20" name="2018"/>
+    <tableColumn id="21" name="2019"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="rule1_results" displayName="rule1_results" ref="A1:B54" headerRowCount="1">
+  <autoFilter ref="A1:B54"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Rule #1 Metric"/>
+    <tableColumn id="2" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6453,4 +6496,2229 @@
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>API Parameter</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2001</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2002</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2003</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2004</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2005</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>2006</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>2007</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>2008</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>2009</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>2010</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>2011</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>2012</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>2014</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>2015</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>2016</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>revenue</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2761983000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3122433000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3932936000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5263699000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>6921000000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8490000000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>10711000000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>14835000000</v>
+      </c>
+      <c r="J2" t="n">
+        <v>19166000000</v>
+      </c>
+      <c r="K2" t="n">
+        <v>24509000000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>34204000000</v>
+      </c>
+      <c r="M2" t="n">
+        <v>48077000000</v>
+      </c>
+      <c r="N2" t="n">
+        <v>61093000000</v>
+      </c>
+      <c r="O2" t="n">
+        <v>74452000000</v>
+      </c>
+      <c r="P2" t="n">
+        <v>88988000000</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>107006000000</v>
+      </c>
+      <c r="R2" t="n">
+        <v>135987000000</v>
+      </c>
+      <c r="S2" t="n">
+        <v>177866000000</v>
+      </c>
+      <c r="T2" t="n">
+        <v>232887000000</v>
+      </c>
+      <c r="U2" t="n">
+        <v>280522000000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>operating_income</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-863880000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-230672000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>64124000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>270595000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>432000000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>479000000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>399000000</v>
+      </c>
+      <c r="I3" t="n">
+        <v>664000000</v>
+      </c>
+      <c r="J3" t="n">
+        <v>818000000</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1231000000</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1406000000</v>
+      </c>
+      <c r="M3" t="n">
+        <v>862000000</v>
+      </c>
+      <c r="N3" t="n">
+        <v>676000000</v>
+      </c>
+      <c r="O3" t="n">
+        <v>745000000</v>
+      </c>
+      <c r="P3" t="n">
+        <v>178000000</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2233000000</v>
+      </c>
+      <c r="R3" t="n">
+        <v>4186000000</v>
+      </c>
+      <c r="S3" t="n">
+        <v>4106000000</v>
+      </c>
+      <c r="T3" t="n">
+        <v>12421000000</v>
+      </c>
+      <c r="U3" t="n">
+        <v>14541000000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>pretax_income</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-150633000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>38988000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>355000000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>428000000</v>
+      </c>
+      <c r="H4" t="n">
+        <v>377000000</v>
+      </c>
+      <c r="I4" t="n">
+        <v>660000000</v>
+      </c>
+      <c r="J4" t="n">
+        <v>901000000</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1161000000</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1497000000</v>
+      </c>
+      <c r="M4" t="n">
+        <v>934000000</v>
+      </c>
+      <c r="N4" t="n">
+        <v>544000000</v>
+      </c>
+      <c r="O4" t="n">
+        <v>506000000</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-111000000</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1568000000</v>
+      </c>
+      <c r="R4" t="n">
+        <v>3892000000</v>
+      </c>
+      <c r="S4" t="n">
+        <v>3806000000</v>
+      </c>
+      <c r="T4" t="n">
+        <v>11261000000</v>
+      </c>
+      <c r="U4" t="n">
+        <v>13976000000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>income_tax</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>700000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-3706000</v>
+      </c>
+      <c r="F5" t="n">
+        <v>233000000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-95000000</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-187000000</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-184000000</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-247000000</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-253000000</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-352000000</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-291000000</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-428000000</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-161000000</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-167000000</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-950000000</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-1425000000</v>
+      </c>
+      <c r="S5" t="n">
+        <v>-769000000</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-1197000000</v>
+      </c>
+      <c r="U5" t="n">
+        <v>-2374000000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>eps_diluted</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-4.02</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-1.56</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.39</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="L6" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.37</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-0.52</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="R6" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="S6" t="n">
+        <v>6.15</v>
+      </c>
+      <c r="T6" t="n">
+        <v>20.14</v>
+      </c>
+      <c r="U6" t="n">
+        <v>23.01</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>shares_diluted</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>350873000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>364211000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>378363000</v>
+      </c>
+      <c r="E7" t="n">
+        <v>419352000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>425000000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>426000000</v>
+      </c>
+      <c r="H7" t="n">
+        <v>424000000</v>
+      </c>
+      <c r="I7" t="n">
+        <v>424000000</v>
+      </c>
+      <c r="J7" t="n">
+        <v>432000000</v>
+      </c>
+      <c r="K7" t="n">
+        <v>442000000</v>
+      </c>
+      <c r="L7" t="n">
+        <v>456000000</v>
+      </c>
+      <c r="M7" t="n">
+        <v>461000000</v>
+      </c>
+      <c r="N7" t="n">
+        <v>453000000</v>
+      </c>
+      <c r="O7" t="n">
+        <v>465000000</v>
+      </c>
+      <c r="P7" t="n">
+        <v>462000000</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>477000000</v>
+      </c>
+      <c r="R7" t="n">
+        <v>484000000</v>
+      </c>
+      <c r="S7" t="n">
+        <v>493000000</v>
+      </c>
+      <c r="T7" t="n">
+        <v>500000000</v>
+      </c>
+      <c r="U7" t="n">
+        <v>504000000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>total_assets</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2135169000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1637547000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1990449000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2162033000</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3248000000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3696000000</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4363000000</v>
+      </c>
+      <c r="I8" t="n">
+        <v>6485000000</v>
+      </c>
+      <c r="J8" t="n">
+        <v>8314000000</v>
+      </c>
+      <c r="K8" t="n">
+        <v>13813000000</v>
+      </c>
+      <c r="L8" t="n">
+        <v>18797000000</v>
+      </c>
+      <c r="M8" t="n">
+        <v>25278000000</v>
+      </c>
+      <c r="N8" t="n">
+        <v>32555000000</v>
+      </c>
+      <c r="O8" t="n">
+        <v>40159000000</v>
+      </c>
+      <c r="P8" t="n">
+        <v>54505000000</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>64747000000</v>
+      </c>
+      <c r="R8" t="n">
+        <v>83402000000</v>
+      </c>
+      <c r="S8" t="n">
+        <v>131310000000</v>
+      </c>
+      <c r="T8" t="n">
+        <v>162648000000</v>
+      </c>
+      <c r="U8" t="n">
+        <v>225248000000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>st_debt</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>16577000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>14992000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>13318000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4216000</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>17000000</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>lt_debt</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2127464000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2156133000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2277305000</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1945439000</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1855000000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1480000000</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1247000000</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1282000000</v>
+      </c>
+      <c r="J10" t="n">
+        <v>409000000</v>
+      </c>
+      <c r="K10" t="n">
+        <v>109000000</v>
+      </c>
+      <c r="L10" t="n">
+        <v>184000000</v>
+      </c>
+      <c r="M10" t="n">
+        <v>255000000</v>
+      </c>
+      <c r="N10" t="n">
+        <v>3084000000</v>
+      </c>
+      <c r="O10" t="n">
+        <v>3191000000</v>
+      </c>
+      <c r="P10" t="n">
+        <v>8265000000</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>8227000000</v>
+      </c>
+      <c r="R10" t="n">
+        <v>7694000000</v>
+      </c>
+      <c r="S10" t="n">
+        <v>24743000000</v>
+      </c>
+      <c r="T10" t="n">
+        <v>23495000000</v>
+      </c>
+      <c r="U10" t="n">
+        <v>23414000000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>total_equity</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-967251000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-1440000000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-1352814000</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1036107000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-227000000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>246000000</v>
+      </c>
+      <c r="H11" t="n">
+        <v>431000000</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1197000000</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2672000000</v>
+      </c>
+      <c r="K11" t="n">
+        <v>5257000000</v>
+      </c>
+      <c r="L11" t="n">
+        <v>6864000000</v>
+      </c>
+      <c r="M11" t="n">
+        <v>7757000000</v>
+      </c>
+      <c r="N11" t="n">
+        <v>8192000000</v>
+      </c>
+      <c r="O11" t="n">
+        <v>9746000000</v>
+      </c>
+      <c r="P11" t="n">
+        <v>10741000000</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>13384000000</v>
+      </c>
+      <c r="R11" t="n">
+        <v>19285000000</v>
+      </c>
+      <c r="S11" t="n">
+        <v>27709000000</v>
+      </c>
+      <c r="T11" t="n">
+        <v>43549000000</v>
+      </c>
+      <c r="U11" t="n">
+        <v>62060000000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>cf_cfo</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-130442000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-119782000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>174291000</v>
+      </c>
+      <c r="E12" t="n">
+        <v>392022000</v>
+      </c>
+      <c r="F12" t="n">
+        <v>566000000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>733000000</v>
+      </c>
+      <c r="H12" t="n">
+        <v>702000000</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1405000000</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1697000000</v>
+      </c>
+      <c r="K12" t="n">
+        <v>3293000000</v>
+      </c>
+      <c r="L12" t="n">
+        <v>3495000000</v>
+      </c>
+      <c r="M12" t="n">
+        <v>3903000000</v>
+      </c>
+      <c r="N12" t="n">
+        <v>4180000000</v>
+      </c>
+      <c r="O12" t="n">
+        <v>5475000000</v>
+      </c>
+      <c r="P12" t="n">
+        <v>6842000000</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>12039000000</v>
+      </c>
+      <c r="R12" t="n">
+        <v>17203000000</v>
+      </c>
+      <c r="S12" t="n">
+        <v>18365000000</v>
+      </c>
+      <c r="T12" t="n">
+        <v>30723000000</v>
+      </c>
+      <c r="U12" t="n">
+        <v>38514000000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cfi_ppe_net</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-134758000</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-50321000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-39163000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-40891000</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-89000000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-204000000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-216000000</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-224000000</v>
+      </c>
+      <c r="J13" t="n">
+        <v>-333000000</v>
+      </c>
+      <c r="K13" t="n">
+        <v>-373000000</v>
+      </c>
+      <c r="L13" t="n">
+        <v>-979000000</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-1811000000</v>
+      </c>
+      <c r="N13" t="n">
+        <v>-3785000000</v>
+      </c>
+      <c r="O13" t="n">
+        <v>-3444000000</v>
+      </c>
+      <c r="P13" t="n">
+        <v>-4893000000</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>-4589000000</v>
+      </c>
+      <c r="R13" t="n">
+        <v>-6737000000</v>
+      </c>
+      <c r="S13" t="n">
+        <v>-10058000000</v>
+      </c>
+      <c r="T13" t="n">
+        <v>-11323000000</v>
+      </c>
+      <c r="U13" t="n">
+        <v>-12689000000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>roic</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-1.4342</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-2.0809</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-0.7639</v>
+      </c>
+      <c r="E14" t="n">
+        <v>6.5156</v>
+      </c>
+      <c r="F14" t="n">
+        <v>8.5047</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.6870000000000001</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.2725</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.3697</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2.8351</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.7213000000000001</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.3977</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.1653</v>
+      </c>
+      <c r="N14" t="n">
+        <v>-0.009900000000000001</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.0536</v>
+      </c>
+      <c r="P14" t="n">
+        <v>-0.0322</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.0585</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.1767</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.1006</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.2237</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.1728</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>revenue_growth</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.6843</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.1305</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.2595</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.3383</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.3148</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.2267</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.2616</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.2919</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.2787</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.3955</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.4055</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.2707</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.2186</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.1952</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.2024</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.2708</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.3079</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.3093</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.2045</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>eps_diluted_growth</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-0.8272</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.6119</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1.2051</v>
+      </c>
+      <c r="F16" t="n">
+        <v>16.375</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-0.3956</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-0.4642</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1.4888</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.3303</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.3691</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.2401</v>
+      </c>
+      <c r="M16" t="n">
+        <v>-0.4584</v>
+      </c>
+      <c r="N16" t="n">
+        <v>-1.0656</v>
+      </c>
+      <c r="O16" t="n">
+        <v>7.5555</v>
+      </c>
+      <c r="P16" t="n">
+        <v>-1.8813</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>3.4038</v>
+      </c>
+      <c r="R16" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.2551</v>
+      </c>
+      <c r="T16" t="n">
+        <v>2.2747</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.1425</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>total_equity_growth</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>-4.6321</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-0.4887</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0605</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.2341</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.7809</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2.0837</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.752</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1.7772</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1.2322</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.9674</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.3056</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.056</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.1896</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.246</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.4408</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.4368</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.5716</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.425</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>cfo_growth</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>-0.435</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.08169999999999999</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.455</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.2492</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.4437</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.295</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-0.0422</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.0014</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.2078</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.9404</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.0613</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.1167</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.0709</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.3098</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.2496</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.7595</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.4289</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.0675</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.6729000000000001</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.2535</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>fcf_growth</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.2984</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.3585</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.7943</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.5985</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.3584</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.109</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-0.08119999999999999</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.1549</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1.1407</v>
+      </c>
+      <c r="L19" t="n">
+        <v>-0.1383</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-0.1685</v>
+      </c>
+      <c r="N19" t="n">
+        <v>-0.8111</v>
+      </c>
+      <c r="O19" t="n">
+        <v>4.1417</v>
+      </c>
+      <c r="P19" t="n">
+        <v>-0.0403</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>2.8224</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.4048</v>
+      </c>
+      <c r="S19" t="n">
+        <v>-0.2062</v>
+      </c>
+      <c r="T19" t="n">
+        <v>1.3353</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.3311</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>fcf</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-265200000</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-170103000</v>
+      </c>
+      <c r="D20" t="n">
+        <v>135128000</v>
+      </c>
+      <c r="E20" t="n">
+        <v>351131000</v>
+      </c>
+      <c r="F20" t="n">
+        <v>477000000</v>
+      </c>
+      <c r="G20" t="n">
+        <v>529000000</v>
+      </c>
+      <c r="H20" t="n">
+        <v>486000000</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1181000000</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1364000000</v>
+      </c>
+      <c r="K20" t="n">
+        <v>2920000000</v>
+      </c>
+      <c r="L20" t="n">
+        <v>2516000000</v>
+      </c>
+      <c r="M20" t="n">
+        <v>2092000000</v>
+      </c>
+      <c r="N20" t="n">
+        <v>395000000</v>
+      </c>
+      <c r="O20" t="n">
+        <v>2031000000</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1949000000</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>7450000000</v>
+      </c>
+      <c r="R20" t="n">
+        <v>10466000000</v>
+      </c>
+      <c r="S20" t="n">
+        <v>8307000000</v>
+      </c>
+      <c r="T20" t="n">
+        <v>19400000000</v>
+      </c>
+      <c r="U20" t="n">
+        <v>25825000000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>book_value_per_share</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-2.7566</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-3.9537</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-3.5754</v>
+      </c>
+      <c r="E21" t="n">
+        <v>-2.4707</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-0.5341</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.5774</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1.0165</v>
+      </c>
+      <c r="I21" t="n">
+        <v>2.8231</v>
+      </c>
+      <c r="J21" t="n">
+        <v>6.1851</v>
+      </c>
+      <c r="K21" t="n">
+        <v>11.8936</v>
+      </c>
+      <c r="L21" t="n">
+        <v>15.0526</v>
+      </c>
+      <c r="M21" t="n">
+        <v>16.8264</v>
+      </c>
+      <c r="N21" t="n">
+        <v>18.0838</v>
+      </c>
+      <c r="O21" t="n">
+        <v>20.9591</v>
+      </c>
+      <c r="P21" t="n">
+        <v>23.2489</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>28.0587</v>
+      </c>
+      <c r="R21" t="n">
+        <v>39.845</v>
+      </c>
+      <c r="S21" t="n">
+        <v>56.2048</v>
+      </c>
+      <c r="T21" t="n">
+        <v>87.098</v>
+      </c>
+      <c r="U21" t="n">
+        <v>123.1349</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>market_cap</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>5557098400</v>
+      </c>
+      <c r="C22" t="n">
+        <v>4038218760</v>
+      </c>
+      <c r="D22" t="n">
+        <v>7327544340</v>
+      </c>
+      <c r="E22" t="n">
+        <v>21224487480</v>
+      </c>
+      <c r="F22" t="n">
+        <v>18146100190</v>
+      </c>
+      <c r="G22" t="n">
+        <v>19614400000</v>
+      </c>
+      <c r="H22" t="n">
+        <v>16336440000</v>
+      </c>
+      <c r="I22" t="n">
+        <v>38538240000</v>
+      </c>
+      <c r="J22" t="n">
+        <v>21977736240</v>
+      </c>
+      <c r="K22" t="n">
+        <v>59726880000</v>
+      </c>
+      <c r="L22" t="n">
+        <v>81180000000</v>
+      </c>
+      <c r="M22" t="n">
+        <v>78760500000</v>
+      </c>
+      <c r="N22" t="n">
+        <v>113894980000</v>
+      </c>
+      <c r="O22" t="n">
+        <v>183044610000</v>
+      </c>
+      <c r="P22" t="n">
+        <v>144312750000</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>318344190000</v>
+      </c>
+      <c r="R22" t="n">
+        <v>357687990000</v>
+      </c>
+      <c r="S22" t="n">
+        <v>566023480000</v>
+      </c>
+      <c r="T22" t="n">
+        <v>737467270000</v>
+      </c>
+      <c r="U22" t="n">
+        <v>920224320000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>price_to_earnings</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>-3.9376</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-7.1186</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-49.1346</v>
+      </c>
+      <c r="E23" t="n">
+        <v>601.567</v>
+      </c>
+      <c r="F23" t="n">
+        <v>30.8607</v>
+      </c>
+      <c r="G23" t="n">
+        <v>54.6362</v>
+      </c>
+      <c r="H23" t="n">
+        <v>85.9812</v>
+      </c>
+      <c r="I23" t="n">
+        <v>80.96259999999999</v>
+      </c>
+      <c r="J23" t="n">
+        <v>34.074</v>
+      </c>
+      <c r="K23" t="n">
+        <v>66.21599999999999</v>
+      </c>
+      <c r="L23" t="n">
+        <v>70.4687</v>
+      </c>
+      <c r="M23" t="n">
+        <v>124.8185</v>
+      </c>
+      <c r="N23" t="n">
+        <v>-2920.3841</v>
+      </c>
+      <c r="O23" t="n">
+        <v>668.046</v>
+      </c>
+      <c r="P23" t="n">
+        <v>-598.808</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>534.1345</v>
+      </c>
+      <c r="R23" t="n">
+        <v>150.8595</v>
+      </c>
+      <c r="S23" t="n">
+        <v>186.6216</v>
+      </c>
+      <c r="T23" t="n">
+        <v>73.2122</v>
+      </c>
+      <c r="U23" t="n">
+        <v>79.4118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Rule #1 Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ROIC - 10-year</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.08104887735672703</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ROIC - 5-year</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.1016671592840285</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ROIC - 3-year</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1230874352485137</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ROIC - 1-year</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1412245550550465</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ROIC QuickFS - 10-year</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.13068</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ROIC QuickFS - 5-year</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.14646</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ROIC QuickFS - 3-year</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1657</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ROIC QuickFS - 1-year</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.1728</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Equity Growth Rate - 10-year</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>26.33%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Equity Growth Rate - 5-year</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>39.57%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Equity Growth Rate - 3-year</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>45.66%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Equity Growth Rate - 1-year</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>41.38%</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>EPS Growth Rate - 10-year</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>27.42%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>EPS Growth Rate - 5-year</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>214.35%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>EPS Growth Rate - 3-year</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>67.46%</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>EPS Growth Rate - 1-year</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>14.25%</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Sales Growth Rate - 10-year</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>27.60%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Sales Growth Rate - 5-year</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>25.81%</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Sales Growth Rate - 3-year</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>27.30%</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Sales Growth Rate - 1-year</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>20.45%</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>FCF Growth Rate - 10-year</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>24.36%</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>FCF Growth Rate - 5-year</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>67.67%</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>FCF Growth Rate - 3-year</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>35.13%</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>FCF Growth Rate - 1-year</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>33.12%</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>OCF Growth Rate - 10-year</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>27.88%</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>OCF Growth Rate - 5-year</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>41.28%</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>OCF Growth Rate - 3-year</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>30.82%</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>OCF Growth Rate - 1-year</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>25.36%</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Debt - Current Long-Term Debt</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>23414000000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Debt - Payoff Possible</t>
+        </is>
+      </c>
+      <c r="B31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>current_eps</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>34.20199898263665</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>analyst_growth_rate</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.3635</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>equity_growth_rate</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.3823371560917213</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>eps_growth_rate</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.3635</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>future_eps</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>759.6314072547541</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>average_historical_pe</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>-163.16193</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>default_pe</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>72.7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>future_pe</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>-163.16193</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>future_market_price</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>-123942.9264963017</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>sticker_price</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>-30636.79586187236</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>margin_of_safety</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>-15318.39793093618</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>shortName</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Amazon.com, Inc.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>market</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>us_market</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>exchange</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>NMS</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sector</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Consumer Cyclical</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>industry</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Internet Retail</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>website</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>http://www.amazon.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>marketCap</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1648678535168</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>volume</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>3209310</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>forwardPE</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>72.35961</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>